<commit_message>
Fixed Formatting of JSON to Create A Clean CSV
</commit_message>
<xml_diff>
--- a/dataFile.xlsx
+++ b/dataFile.xlsx
@@ -434,438 +434,444 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="n">
-        <v>2</v>
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Price</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Symbol</t>
+        </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>{'Symbol': 'BTC-USD'}</t>
+          <t>23,788.94</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>{'Name': 'Bitcoin USD'}</t>
+          <t>Bitcoin USD</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>{'Price': '23,736.93'}</t>
+          <t>BTC-USD</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>{'Symbol': 'ETH-USD'}</t>
+          <t>1,769.95</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>{'Name': 'Ethereum USD'}</t>
+          <t>Ethereum USD</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>{'Price': '1,768.13'}</t>
+          <t>ETH-USD</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>{'Symbol': 'USDT-USD'}</t>
+          <t>1.0002</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>{'Name': 'Tether USD'}</t>
+          <t>Tether USD</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>{'Price': '1.0002'}</t>
+          <t>USDT-USD</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>{'Symbol': 'USDC-USD'}</t>
+          <t>0.999945</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>{'Name': 'USD Coin USD'}</t>
+          <t>USD Coin USD</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{'Price': '1.0000'}</t>
+          <t>USDC-USD</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>{'Symbol': 'BNB-USD'}</t>
+          <t>324.47</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>{'Name': 'Binance Coin USD'}</t>
+          <t>Binance Coin USD</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{'Price': '324.76'}</t>
+          <t>BNB-USD</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>{'Symbol': 'XRP-USD'}</t>
+          <t>0.376197</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>{'Name': 'XRP USD'}</t>
+          <t>XRP USD</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{'Price': '0.375768'}</t>
+          <t>XRP-USD</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>{'Symbol': 'ADA-USD'}</t>
+          <t>0.533140</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>{'Name': 'Cardano USD'}</t>
+          <t>Cardano USD</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>{'Price': '0.529881'}</t>
+          <t>ADA-USD</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>{'Symbol': 'BUSD-USD'}</t>
+          <t>0.999966</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>{'Name': 'Binance USD USD'}</t>
+          <t>Binance USD USD</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>{'Price': '1.0002'}</t>
+          <t>BUSD-USD</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>{'Symbol': 'SOL-USD'}</t>
+          <t>42.32</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>{'Name': 'Solana USD'}</t>
+          <t>Solana USD</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{'Price': '41.78'}</t>
+          <t>SOL-USD</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>{'Symbol': 'DOT-USD'}</t>
+          <t>9.1351</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>{'Name': 'Polkadot USD'}</t>
+          <t>Polkadot USD</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{'Price': '9.1354'}</t>
+          <t>DOT-USD</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>{'Symbol': 'DOGE-USD'}</t>
+          <t>0.071363</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>{'Name': 'Dogecoin USD'}</t>
+          <t>Dogecoin USD</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{'Price': '0.070005'}</t>
+          <t>DOGE-USD</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>{'Symbol': 'HEX-USD'}</t>
+          <t>0.053941</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>{'Name': 'HEX USD'}</t>
+          <t>HEX USD</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{'Price': '0.053433'}</t>
+          <t>HEX-USD</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>{'Symbol': 'AVAX-USD'}</t>
+          <t>28.35</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>{'Name': 'Avalanche USD'}</t>
+          <t>Avalanche USD</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>{'Price': '27.73'}</t>
+          <t>AVAX-USD</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>{'Symbol': 'DAI-USD'}</t>
+          <t>0.999564</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>{'Name': 'Dai USD'}</t>
+          <t>Dai USD</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>{'Price': '0.999913'}</t>
+          <t>DAI-USD</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>{'Symbol': 'MATIC-USD'}</t>
+          <t>0.923054</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>{'Name': 'Polygon USD'}</t>
+          <t>Polygon USD</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>{'Price': '0.918632'}</t>
+          <t>MATIC-USD</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>{'Symbol': 'WTRX-USD'}</t>
+          <t>0.070251</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>{'Name': 'Wrapped TRON USD'}</t>
+          <t>Wrapped TRON USD</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>{'Price': '0.070001'}</t>
+          <t>WTRX-USD</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>{'Symbol': 'STA-USD'}</t>
+          <t>0.000012</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>{'Name': 'STATERA USD'}</t>
+          <t>SHIBA INU USD</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>{'Price': '85.69'}</t>
+          <t>SHIB-USD</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>{'Symbol': 'SHIB-USD'}</t>
+          <t>85.84</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>{'Name': 'SHIBA INU USD'}</t>
+          <t>STATERA USD</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>{'Price': '0.000012'}</t>
+          <t>STA-USD</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>{'Symbol': 'UNI1-USD'}</t>
+          <t>8.7848</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>{'Name': 'Uniswap USD'}</t>
+          <t>Uniswap USD</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>{'Price': '8.7901'}</t>
+          <t>UNI1-USD</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>{'Symbol': 'TRX-USD'}</t>
+          <t>0.070231</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>{'Name': 'TRON USD'}</t>
+          <t>TRON USD</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>{'Price': '0.070049'}</t>
+          <t>TRX-USD</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>{'Symbol': 'STETH-USD'}</t>
+          <t>1,709.10</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>{'Name': 'Lido stETH USD'}</t>
+          <t>Lido stETH USD</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>{'Price': '1,705.70'}</t>
+          <t>STETH-USD</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>{'Symbol': 'WBTC-USD'}</t>
+          <t>23,799.38</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>{'Name': 'Wrapped Bitcoin USD'}</t>
+          <t>Wrapped Bitcoin USD</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>{'Price': '23,730.84'}</t>
+          <t>WBTC-USD</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>{'Symbol': 'ETC-USD'}</t>
+          <t>37.75</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>{'Name': 'Ethereum Classic USD'}</t>
+          <t>Ethereum Classic USD</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>{'Price': '37.71'}</t>
+          <t>ETC-USD</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>{'Symbol': 'LEO-USD'}</t>
+          <t>4.7958</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>{'Name': 'UNUS SED LEO USD'}</t>
+          <t>UNUS SED LEO USD</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>{'Price': '4.7908'}</t>
+          <t>LEO-USD</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>{'Symbol': 'LTC-USD'}</t>
+          <t>62.43</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>{'Name': 'Litecoin USD'}</t>
+          <t>Litecoin USD</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>{'Price': '62.21'}</t>
+          <t>LTC-USD</t>
         </is>
       </c>
     </row>

</xml_diff>